<commit_message>
Save report to db
</commit_message>
<xml_diff>
--- a/api/test/test_data.xlsx
+++ b/api/test/test_data.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Ref</t>
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>1/08/2018</t>
   </si>
 </sst>
 </file>
@@ -360,52 +366,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>
       <c r="B2">
         <v>2000</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>251</v>
       </c>
       <c r="B3">
         <v>2500</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>125</v>
-      </c>
-      <c r="B4">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>282</v>
-      </c>
-      <c r="B5">
-        <v>4000</v>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get Existing Payment for the same payment month
</commit_message>
<xml_diff>
--- a/api/test/test_data.xlsx
+++ b/api/test/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\flat\api\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7F3AF830-7610-453C-85E2-685662D39D5D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9885D33D-6158-4506-B255-ACD115F52FC8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,10 +415,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -433,7 +437,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123</v>
+        <v>2020</v>
       </c>
       <c r="B2">
         <v>2000</v>
@@ -444,7 +448,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>251</v>
+        <v>2019</v>
       </c>
       <c r="B3">
         <v>2500</v>
@@ -455,7 +459,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>222</v>
+        <v>2018</v>
       </c>
       <c r="B4">
         <v>1500</v>

</xml_diff>